<commit_message>
Entry Parser tested and Works
</commit_message>
<xml_diff>
--- a/Documentation/Design Analysis/ActivityParserAnalysis.xlsx
+++ b/Documentation/Design Analysis/ActivityParserAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theod\Documents\Git\WeeklyReview\Documentation\Design Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CBE3E2-E99E-4EEE-ADF9-2EB6CC4EEFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AFB94A-A366-44BD-A7B8-8672CD485F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{80ABE21A-6301-4AD2-9AE9-C826E7C7742E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
   <si>
     <t>Input</t>
   </si>
@@ -167,12 +167,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -191,8 +190,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D7B774BD-1023-4FC9-A7CE-E2A13BFC76A5}" name="Table1" displayName="Table1" ref="A2:F13" totalsRowShown="0">
-  <autoFilter ref="A2:F13" xr:uid="{D7B774BD-1023-4FC9-A7CE-E2A13BFC76A5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D7B774BD-1023-4FC9-A7CE-E2A13BFC76A5}" name="Table1" displayName="Table1" ref="A2:F14" totalsRowShown="0">
+  <autoFilter ref="A2:F14" xr:uid="{D7B774BD-1023-4FC9-A7CE-E2A13BFC76A5}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{18753B61-E989-4474-A322-FE428F368CA0}" name="Input 1"/>
     <tableColumn id="2" xr3:uid="{2F0DE260-BCF8-4C3E-A7B9-A005F0EB4BE6}" name="Input 2"/>
@@ -514,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C61E607-F670-4C5E-B773-B65A1EE03034}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,18 +737,26 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Added cases where activity and category does not exist
</commit_message>
<xml_diff>
--- a/Documentation/Design Analysis/ActivityParserAnalysis.xlsx
+++ b/Documentation/Design Analysis/ActivityParserAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theod\Documents\Git\WeeklyReview\Documentation\Design Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AFB94A-A366-44BD-A7B8-8672CD485F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBA45B7-1164-443B-B550-FA4AD694975A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{80ABE21A-6301-4AD2-9AE9-C826E7C7742E}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>Input</t>
   </si>
   <si>
-    <t>Bike</t>
-  </si>
-  <si>
     <t>Sports: Bike</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>Exercise: Bike</t>
   </si>
   <si>
-    <t>Exercise, Run</t>
-  </si>
-  <si>
     <t>Sports:</t>
   </si>
   <si>
@@ -132,6 +126,9 @@
   </si>
   <si>
     <t>Difficult Competions: Participating in Race</t>
+  </si>
+  <si>
+    <t>Exercise, Bike</t>
   </si>
 </sst>
 </file>
@@ -205,8 +202,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D5A627A1-5A07-4957-A134-07424E1D843E}" name="Table2" displayName="Table2" ref="H2:J7" totalsRowShown="0">
-  <autoFilter ref="H2:J7" xr:uid="{D5A627A1-5A07-4957-A134-07424E1D843E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D5A627A1-5A07-4957-A134-07424E1D843E}" name="Table2" displayName="Table2" ref="H2:J6" totalsRowShown="0">
+  <autoFilter ref="H2:J6" xr:uid="{D5A627A1-5A07-4957-A134-07424E1D843E}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{44F6B6D6-BB4F-4A63-955F-E0F51FC7F930}" name="Input"/>
     <tableColumn id="2" xr3:uid="{C0707C9C-7C25-4A66-B7D7-9F4B2080786A}" name="Exists"/>
@@ -515,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C61E607-F670-4C5E-B773-B65A1EE03034}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +530,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -541,221 +538,212 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
       </c>
       <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
         <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
         <v>29</v>
-      </c>
-      <c r="D13" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Category duplication bug
</commit_message>
<xml_diff>
--- a/Documentation/Design Analysis/ActivityParserAnalysis.xlsx
+++ b/Documentation/Design Analysis/ActivityParserAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theod\Documents\Git\WeeklyReview\Documentation\Design Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302AE67D-5C73-4F1C-8717-EFF484035F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DF5219-575B-4265-B4BE-795F18F24943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{80ABE21A-6301-4AD2-9AE9-C826E7C7742E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{80ABE21A-6301-4AD2-9AE9-C826E7C7742E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
   <si>
     <t>Input</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>[Default, which is empty]</t>
+  </si>
+  <si>
+    <t>Exercise: Bike, Exercise: Run</t>
+  </si>
+  <si>
+    <t>Exercise, Bike, Run</t>
   </si>
 </sst>
 </file>
@@ -205,8 +211,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D5A627A1-5A07-4957-A134-07424E1D843E}" name="Table2" displayName="Table2" ref="H2:J7" totalsRowShown="0">
-  <autoFilter ref="H2:J7" xr:uid="{D5A627A1-5A07-4957-A134-07424E1D843E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D5A627A1-5A07-4957-A134-07424E1D843E}" name="Table2" displayName="Table2" ref="H2:J8" totalsRowShown="0">
+  <autoFilter ref="H2:J8" xr:uid="{D5A627A1-5A07-4957-A134-07424E1D843E}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{44F6B6D6-BB4F-4A63-955F-E0F51FC7F930}" name="Input"/>
     <tableColumn id="2" xr3:uid="{C0707C9C-7C25-4A66-B7D7-9F4B2080786A}" name="Exists"/>
@@ -516,7 +522,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,6 +535,7 @@
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -634,7 +641,10 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>8</v>
+        <v>32</v>
+      </c>
+      <c r="J6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -654,13 +664,7 @@
         <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -681,6 +685,15 @@
       </c>
       <c r="F8" t="s">
         <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>